<commit_message>
Keyword Driven done Signed-off-by: evnraja32 <evnraja32@gmail.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/data/KeywordsExcel.xlsx
+++ b/src/main/resources/data/KeywordsExcel.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="25">
   <si>
     <t>Funcationality</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>chrome</t>
+  </si>
+  <si>
+    <t>mYdUhUpIl</t>
   </si>
 </sst>
 </file>
@@ -756,7 +759,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,7 +827,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2"/>
     </row>

</xml_diff>